<commit_message>
EAP atualizado conforme orientações. Pendente formatar documento segundo abnt 2023
</commit_message>
<xml_diff>
--- a/3DES/PROJ/AULA06/orcamento.xlsx
+++ b/3DES/PROJ/AULA06/orcamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desenvolvimento\Desktop\SENAI\3DES\PROJ\AULA06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C206B640-D14C-4283-875E-4FB6E10E8720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658A811F-58B1-4270-970C-15F805950FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{211DDD06-3D26-4092-BDF8-45B9ACFDDFF6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Valor/Hora</t>
   </si>
@@ -97,6 +97,81 @@
   </si>
   <si>
     <t>Tarefas realizadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Criação do script sql</t>
+  </si>
+  <si>
+    <t>Mobile - Estruturação - Tela de Login</t>
+  </si>
+  <si>
+    <t>Mobile - Estruturação - Tela de Gestão - Modificar situação atual do veículo</t>
+  </si>
+  <si>
+    <t>Mobile - Estruturação - Tela de Gestão - Relatório de disponibilidade</t>
+  </si>
+  <si>
+    <t>Mobile - Estruturação - Tela de Gestão - Relatório de manutenção</t>
+  </si>
+  <si>
+    <t>Mobile - Estilização - Tela de Login</t>
+  </si>
+  <si>
+    <t>Mobile - Estilização - Tela de Gestão - veículos</t>
+  </si>
+  <si>
+    <t>Mobile - Estilização - Tela de Gestão - Relatórios</t>
+  </si>
+  <si>
+    <t>Web - Estilização - Interface relatórios</t>
+  </si>
+  <si>
+    <t>Web - Estilização - Interface de gerenciamento das operações</t>
+  </si>
+  <si>
+    <t>Web - Estilização - Interface de gerenciamento das manutenções</t>
+  </si>
+  <si>
+    <t>Web - Estilização - Interface de gerenciamento dos veículos</t>
+  </si>
+  <si>
+    <t>Web - Estrutura e estilização - Página de Login</t>
+  </si>
+  <si>
+    <t>Web - Estilização - Interface de gerenciamento dos motoristas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back - Desenvolvimento do CRUD referente a tabela usuários(login) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back - Desenvolvimento do CRUD referente a tabela motoristas </t>
+  </si>
+  <si>
+    <t>Back - Desenvolvimento do CRUD referente a tabela veículos</t>
+  </si>
+  <si>
+    <t>Back - Desenvolvimento do CRUD referente a tabela manutenções</t>
+  </si>
+  <si>
+    <t>Back - Desenvolvimento do CRUD referente a tabela operações</t>
+  </si>
+  <si>
+    <t>Web - Estruturação - Interface de gerenciamento dos motoristas</t>
+  </si>
+  <si>
+    <t>Web - Estruturação - Interface de gerenciamento dos veículos</t>
+  </si>
+  <si>
+    <t>Web - Estruturação - Interface de gerenciamento das manutenções</t>
+  </si>
+  <si>
+    <t>Web - Estruturação - Interface de gerenciamento das operações</t>
+  </si>
+  <si>
+    <t>Web - Estruturação - Interface relatórios</t>
   </si>
 </sst>
 </file>
@@ -107,7 +182,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,13 +208,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -302,12 +370,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -323,7 +391,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -642,7 +712,7 @@
   <dimension ref="B2:I13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +757,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="9">
-        <f>$F$3*C3</f>
+        <f t="shared" ref="D3:D8" si="0">$F$3*C3</f>
         <v>320.39999999999998</v>
       </c>
       <c r="F3" s="4">
@@ -714,7 +784,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="11">
-        <f>$F$3*C4</f>
+        <f t="shared" si="0"/>
         <v>453.9</v>
       </c>
     </row>
@@ -726,7 +796,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="9">
-        <f>$F$3*C5</f>
+        <f t="shared" si="0"/>
         <v>453.9</v>
       </c>
     </row>
@@ -738,7 +808,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="11">
-        <f>$F$3*C6</f>
+        <f t="shared" si="0"/>
         <v>587.4</v>
       </c>
     </row>
@@ -750,7 +820,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="9">
-        <f>$F$3*C7</f>
+        <f t="shared" si="0"/>
         <v>587.4</v>
       </c>
     </row>
@@ -762,7 +832,7 @@
         <v>30</v>
       </c>
       <c r="D8" s="11">
-        <f>$F$3*C8</f>
+        <f t="shared" si="0"/>
         <v>801</v>
       </c>
     </row>
@@ -803,21 +873,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFC5B09-AF59-4288-8FB1-3ED32641577E}">
-  <dimension ref="B2:AE12"/>
+  <dimension ref="B2:XFD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI20" sqref="AI20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="14" width="3" bestFit="1" customWidth="1"/>
     <col min="15" max="23" width="3" customWidth="1"/>
     <col min="24" max="31" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
         <v>14</v>
       </c>
@@ -853,7 +923,7 @@
       <c r="AD2" s="22"/>
       <c r="AE2" s="22"/>
     </row>
-    <row r="3" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
       <c r="B3" s="24"/>
       <c r="C3" s="21" t="s">
         <v>16</v>
@@ -889,7 +959,7 @@
       <c r="AD3" s="21"/>
       <c r="AE3" s="21"/>
     </row>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
       <c r="B4" s="25"/>
       <c r="C4" s="14">
         <v>17</v>
@@ -979,14 +1049,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
       <c r="I5" s="15"/>
@@ -1013,21 +1083,21 @@
       <c r="AD5" s="15"/>
       <c r="AE5" s="15"/>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+        <v>35</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="16"/>
       <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
       <c r="P6" s="15"/>
@@ -1047,28 +1117,28 @@
       <c r="AD6" s="15"/>
       <c r="AE6" s="15"/>
     </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="19"/>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="19"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="19"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
       <c r="U7" s="15"/>
       <c r="V7" s="15"/>
       <c r="W7" s="15"/>
@@ -1081,18 +1151,18 @@
       <c r="AD7" s="15"/>
       <c r="AE7" s="15"/>
     </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="19"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
@@ -1100,24 +1170,24 @@
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="19"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="19"/>
-      <c r="Z8" s="19"/>
-      <c r="AA8" s="19"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
       <c r="AB8" s="15"/>
       <c r="AC8" s="15"/>
       <c r="AD8" s="15"/>
       <c r="AE8" s="15"/>
     </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -1125,8 +1195,8 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
@@ -1138,20 +1208,20 @@
       <c r="S9" s="15"/>
       <c r="T9" s="15"/>
       <c r="U9" s="15"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="20"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
       <c r="AA9" s="15"/>
       <c r="AB9" s="15"/>
       <c r="AC9" s="15"/>
       <c r="AD9" s="15"/>
       <c r="AE9" s="15"/>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -1160,8 +1230,8 @@
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
@@ -1172,28 +1242,646 @@
       <c r="S10" s="15"/>
       <c r="T10" s="15"/>
       <c r="U10" s="15"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="19"/>
-      <c r="AA10" s="16"/>
-      <c r="AB10" s="16"/>
-      <c r="AC10" s="16"/>
-      <c r="AD10" s="20"/>
-      <c r="AE10" s="20"/>
-    </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
+      <c r="Z10" s="15"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="15"/>
+      <c r="AD10" s="15"/>
+      <c r="AE10" s="15"/>
+      <c r="XFD10" s="15"/>
+    </row>
+    <row r="11" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B11" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
+      <c r="AA11" s="15"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="15"/>
+    </row>
+    <row r="12" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="15"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="15"/>
+      <c r="AE12" s="15"/>
+    </row>
+    <row r="13" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="15"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="15"/>
+      <c r="AD13" s="15"/>
+      <c r="AE13" s="15"/>
+    </row>
+    <row r="14" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
+    </row>
+    <row r="15" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+      <c r="X15" s="15"/>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="15"/>
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="15"/>
+      <c r="AC15" s="15"/>
+      <c r="AD15" s="15"/>
+      <c r="AE15" s="15"/>
+    </row>
+    <row r="16" spans="2:31 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
+      <c r="AD16" s="15"/>
+      <c r="AE16" s="15"/>
+    </row>
+    <row r="17" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="15"/>
+      <c r="AB17" s="15"/>
+      <c r="AC17" s="15"/>
+      <c r="AD17" s="15"/>
+      <c r="AE17" s="15"/>
+    </row>
+    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="15"/>
+      <c r="AC18" s="15"/>
+      <c r="AD18" s="15"/>
+      <c r="AE18" s="15"/>
+    </row>
+    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="15"/>
+      <c r="AB19" s="15"/>
+      <c r="AC19" s="15"/>
+      <c r="AD19" s="15"/>
+      <c r="AE19" s="15"/>
+    </row>
+    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="15"/>
+      <c r="AD20" s="15"/>
+      <c r="AE20" s="15"/>
+    </row>
+    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="15"/>
+      <c r="Z21" s="15"/>
+      <c r="AA21" s="15"/>
+      <c r="AB21" s="15"/>
+      <c r="AC21" s="15"/>
+      <c r="AD21" s="15"/>
+      <c r="AE21" s="15"/>
+    </row>
+    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" s="15"/>
+      <c r="AB22" s="15"/>
+      <c r="AC22" s="15"/>
+      <c r="AD22" s="15"/>
+      <c r="AE22" s="15"/>
+    </row>
+    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="15"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="15"/>
+      <c r="AB23" s="15"/>
+      <c r="AC23" s="15"/>
+      <c r="AD23" s="15"/>
+      <c r="AE23" s="15"/>
+    </row>
+    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+      <c r="X24" s="16"/>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="15"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="15"/>
+      <c r="AE24" s="15"/>
+    </row>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="15"/>
+      <c r="X25" s="15"/>
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="15"/>
+      <c r="AA25" s="15"/>
+      <c r="AB25" s="15"/>
+      <c r="AC25" s="15"/>
+      <c r="AD25" s="15"/>
+      <c r="AE25" s="15"/>
+    </row>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="15"/>
+      <c r="X26" s="15"/>
+      <c r="Y26" s="15"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="15"/>
+      <c r="AB26" s="15"/>
+      <c r="AC26" s="15"/>
+      <c r="AD26" s="15"/>
+      <c r="AE26" s="15"/>
+    </row>
+    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="15"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="15"/>
+      <c r="X27" s="15"/>
+      <c r="Y27" s="15"/>
+      <c r="Z27" s="15"/>
+      <c r="AA27" s="16"/>
+      <c r="AB27" s="16"/>
+      <c r="AC27" s="15"/>
+      <c r="AD27" s="15"/>
+      <c r="AE27" s="15"/>
+    </row>
+    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
+      <c r="X28" s="15"/>
+      <c r="Y28" s="15"/>
+      <c r="Z28" s="15"/>
+      <c r="AA28" s="15"/>
+      <c r="AB28" s="15"/>
+      <c r="AC28" s="16"/>
+      <c r="AD28" s="16"/>
+      <c r="AE28" s="15"/>
+    </row>
+    <row r="29" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="18"/>
-    </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
+      <c r="C29" s="18"/>
+    </row>
+    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="26"/>
+      <c r="C30" s="20"/>
+    </row>
+    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O34" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1203,5 +1891,6 @@
     <mergeCell ref="B2:B4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>